<commit_message>
Fixed the browser invoke and added login method in page action package
</commit_message>
<xml_diff>
--- a/openmrs/src/main/resources/PASSDATA/PassData_Configuration.xlsx
+++ b/openmrs/src/main/resources/PASSDATA/PassData_Configuration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -106,10 +106,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -414,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +451,7 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -464,7 +465,7 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -481,7 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Database query helper
</commit_message>
<xml_diff>
--- a/openmrs/src/main/resources/PASSDATA/PassData_Configuration.xlsx
+++ b/openmrs/src/main/resources/PASSDATA/PassData_Configuration.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Environment</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Chrome</t>
+  </si>
+  <si>
+    <t>http://demo.guru99.com/V4/</t>
+  </si>
+  <si>
+    <t>Imps</t>
+  </si>
+  <si>
+    <t>mngr241185</t>
+  </si>
+  <si>
+    <t>vanurEh</t>
   </si>
 </sst>
 </file>
@@ -413,17 +425,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -469,10 +481,25 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -483,7 +510,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +534,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>

</xml_diff>